<commit_message>
Created notebook to combine 2000 to 2004 data files and generate combined .csv.
</commit_message>
<xml_diff>
--- a/Data/Team_Stats/Defense File Column Names.xlsx
+++ b/Data/Team_Stats/Defense File Column Names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06e891e7ad7d67e2/Rutgers Bootcamp/Projects/Final Project/Repository/Data/Team_Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEEA1A41-86FB-4029-9D12-E1F0CCE94CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{CEEA1A41-86FB-4029-9D12-E1F0CCE94CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8897796-42DF-423B-B68D-13AA776A6F46}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="180" windowWidth="25600" windowHeight="10400" xr2:uid="{E17E4333-F3F9-4822-B00E-B6D77D1B94BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{E17E4333-F3F9-4822-B00E-B6D77D1B94BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Year_Def</t>
   </si>
@@ -126,6 +126,105 @@
   </si>
   <si>
     <t>EXP_Def</t>
+  </si>
+  <si>
+    <t>DEFENSE</t>
+  </si>
+  <si>
+    <t>OFFENSE</t>
+  </si>
+  <si>
+    <t>Year_Off</t>
+  </si>
+  <si>
+    <t>Rk_Off</t>
+  </si>
+  <si>
+    <t>Tm_Off</t>
+  </si>
+  <si>
+    <t>Win_Off</t>
+  </si>
+  <si>
+    <t>Loss_Off</t>
+  </si>
+  <si>
+    <t>G_Off</t>
+  </si>
+  <si>
+    <t>PF_Off</t>
+  </si>
+  <si>
+    <t>Total Yds_Off</t>
+  </si>
+  <si>
+    <t>Plays_Off</t>
+  </si>
+  <si>
+    <t>Y/P_Off</t>
+  </si>
+  <si>
+    <t>TO_Off</t>
+  </si>
+  <si>
+    <t>FL_Off</t>
+  </si>
+  <si>
+    <t>1stD_Off</t>
+  </si>
+  <si>
+    <t>Cmp_Off</t>
+  </si>
+  <si>
+    <t>Pass Att_Off</t>
+  </si>
+  <si>
+    <t>Pass Yds_Off</t>
+  </si>
+  <si>
+    <t>Pass TD_Off</t>
+  </si>
+  <si>
+    <t>Int_Off</t>
+  </si>
+  <si>
+    <t>Pass NY/A_Off</t>
+  </si>
+  <si>
+    <t>Pass 1stD_Off</t>
+  </si>
+  <si>
+    <t>Rush Att_Off</t>
+  </si>
+  <si>
+    <t>Rush Yds_Off</t>
+  </si>
+  <si>
+    <t>Rush TD_Off</t>
+  </si>
+  <si>
+    <t>Rush Y/A_Off</t>
+  </si>
+  <si>
+    <t>Rush 1stD_Off</t>
+  </si>
+  <si>
+    <t>Pen_Off</t>
+  </si>
+  <si>
+    <t>Pen Yds_Off</t>
+  </si>
+  <si>
+    <t>1stPy_Off</t>
+  </si>
+  <si>
+    <t>Sc%_Off</t>
+  </si>
+  <si>
+    <t>TO%_Off</t>
+  </si>
+  <si>
+    <t>EXP_Off</t>
   </si>
 </sst>
 </file>
@@ -477,105 +576,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489EB313-044B-44BF-9089-791073CB42BB}">
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>